<commit_message>
Update analysis and add new mgmt scenarios
</commit_message>
<xml_diff>
--- a/Models/Inputs/management_scenarios/new scenarios prioritize pillar.xlsx
+++ b/Models/Inputs/management_scenarios/new scenarios prioritize pillar.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\Research\TCSI conservation finance\Models\Inputs\management_scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swflake\Documents\TCSI-conservation-finance\Models\Inputs\management_scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90F24039-10C6-42CE-B57A-D055417451E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="2625" windowWidth="15360" windowHeight="9360" xr2:uid="{3EDC2C11-82F6-48B8-9EB3-22FBBA12C335}"/>
+    <workbookView xWindow="4230" yWindow="2625" windowWidth="15360" windowHeight="9360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -417,11 +416,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB15EF4B-9F6B-46B1-8FEA-EB05F7CEBE1D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +462,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -480,7 +479,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -497,7 +496,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -514,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -531,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -548,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -565,7 +564,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -582,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -599,7 +598,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -616,7 +615,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -633,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -650,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -667,7 +666,7 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -684,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -701,7 +700,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -718,7 +717,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -735,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -752,7 +751,7 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -769,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -786,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -803,7 +802,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -820,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -837,7 +836,7 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -854,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -871,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -888,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -905,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -922,7 +921,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -939,7 +938,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -956,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -973,7 +972,7 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -990,7 +989,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1007,7 +1006,7 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1024,7 +1023,7 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1041,7 +1040,7 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1058,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1075,7 +1074,7 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1092,7 +1091,7 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1109,7 +1108,7 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1126,7 +1125,7 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1143,7 +1142,7 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1160,7 +1159,7 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1177,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1194,7 +1193,7 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1211,7 +1210,7 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1228,7 +1227,7 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1245,7 +1244,7 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1262,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="E49">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1279,7 +1278,7 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1296,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1313,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1330,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1347,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="E54">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1364,7 +1363,7 @@
         <v>0</v>
       </c>
       <c r="E55">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>